<commit_message>
Barisal 2017 data compiled #3
</commit_message>
<xml_diff>
--- a/Datasets/brri-datasets/barisal_2017-2020/xl_sheets/Barisal Jan -jun 17_R-3-converted.xlsx
+++ b/Datasets/brri-datasets/barisal_2017-2020/xl_sheets/Barisal Jan -jun 17_R-3-converted.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Study Materials\13. Fall 2021\CSE 498R\Weather-Prediction-ML\Datasets\brri-datasets\barisal_2017-2020\xl_sheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5310F80F-AB2F-4EF0-B159-77B01D902B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -14,109 +20,121 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <r>
       <rPr>
-        <sz val="7.0"/>
-        <rFont val="Carlito"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
         <family val="2"/>
+        <charset val="204"/>
       </rPr>
-      <t xml:space="preserve">Solar radition (cal/cm2)</t>
+      <t>Solar radition (cal/cm2)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="6.5"/>
-        <rFont val="Arial"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
         <family val="2"/>
+        <charset val="204"/>
       </rPr>
-      <t xml:space="preserve">Day</t>
+      <t>Day</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="7.0"/>
-        <rFont val="Carlito"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
         <family val="2"/>
+        <charset val="204"/>
       </rPr>
-      <t xml:space="preserve">January</t>
+      <t>January</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="7.0"/>
-        <rFont val="Carlito"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
         <family val="2"/>
+        <charset val="204"/>
       </rPr>
-      <t xml:space="preserve">February</t>
+      <t>February</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="7.0"/>
-        <rFont val="Carlito"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
         <family val="2"/>
+        <charset val="204"/>
       </rPr>
-      <t xml:space="preserve">March</t>
+      <t>March</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="7.0"/>
-        <rFont val="Carlito"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
         <family val="2"/>
+        <charset val="204"/>
       </rPr>
-      <t xml:space="preserve">April</t>
+      <t>April</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="7.0"/>
-        <rFont val="Carlito"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
         <family val="2"/>
+        <charset val="204"/>
       </rPr>
-      <t xml:space="preserve">May</t>
+      <t>May</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="7.0"/>
-        <rFont val="Carlito"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
         <family val="2"/>
+        <charset val="204"/>
       </rPr>
-      <t xml:space="preserve">June</t>
+      <t>June</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="7.0"/>
-        <rFont val="Carlito"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
         <family val="2"/>
+        <charset val="204"/>
       </rPr>
-      <t xml:space="preserve">509.0.3</t>
+      <t>509.0.3</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="0"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -124,18 +142,11 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="7"/>
-      <name val="Carlito"/>
-    </font>
-    <font>
-      <sz val="6.5"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="7"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Carlito"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,7 +157,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -154,105 +165,30 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fillId="0" borderId="0" fontId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fillId="0" borderId="1" fontId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fillId="0" borderId="1" fontId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="9" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fillId="0" borderId="2" fontId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="9" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fillId="0" borderId="3" fontId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="9" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fillId="0" borderId="4" fontId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="9" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fillId="0" borderId="1" fontId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fillId="0" borderId="1" fontId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fillId="0" borderId="1" fontId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fillId="0" borderId="1" fontId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fillId="0" borderId="1" fontId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fillId="0" borderId="1" fontId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -299,7 +235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -331,9 +267,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -365,6 +319,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -540,758 +512,754 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="1" width="5.111111"/>
-    <col min="2" max="2" customWidth="1" width="7.555556"/>
-    <col min="3" max="3" customWidth="1" width="7.777778"/>
-    <col min="4" max="4" customWidth="1" width="7.555556"/>
-    <col min="5" max="5" customWidth="1" width="7.777778"/>
-    <col min="6" max="6" customWidth="1" width="7.777778"/>
-    <col min="7" max="7" customWidth="1" width="7.555556"/>
+    <col min="1" max="1" width="5.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="7.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A3" s="8">
+    <row r="3" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="9">
-        <v>277.72</v>
-      </c>
-      <c r="C3" s="9">
-        <v>32.63</v>
-      </c>
-      <c r="D3" s="9">
+      <c r="B3" s="1">
+        <v>277.72000000000003</v>
+      </c>
+      <c r="C3" s="1">
+        <v>32.630000000000003</v>
+      </c>
+      <c r="D3" s="1">
         <v>428.65</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="1">
         <v>458.61</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="1">
         <v>486.25</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="1">
         <v>282.68</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A4" s="8">
+    <row r="4" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="1">
         <v>257.52</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="1">
         <v>338.38</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="1">
         <v>396.84</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="1">
         <v>461.85</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="1">
         <v>489.5</v>
       </c>
-      <c r="G4" s="9">
-        <v>314.91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A5" s="8">
+      <c r="G4" s="1">
+        <v>314.91000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="1">
         <v>275.2</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="1">
         <v>338.38</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="1">
         <v>406.38</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="1">
         <v>358.34</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="1">
         <v>473.23</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="1">
         <v>479.31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A6" s="8">
+    <row r="6" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="9">
-        <v>277.72</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="B6" s="1">
+        <v>277.72000000000003</v>
+      </c>
+      <c r="C6" s="1">
         <v>347</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="1">
         <v>384.11</v>
       </c>
-      <c r="E6" s="9">
-        <v>316.29</v>
-      </c>
-      <c r="F6" s="10">
+      <c r="E6" s="1">
+        <v>316.29000000000002</v>
+      </c>
+      <c r="F6" s="1">
         <v>489.5</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="1">
         <v>363.26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A7" s="8">
+    <row r="7" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="1">
         <v>219.63</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="1">
         <v>358.5</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="1">
         <v>352.3</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="1">
         <v>397.15</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="1">
         <v>411.38</v>
       </c>
-      <c r="G7" s="10">
-        <v>285.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A8" s="8">
+      <c r="G7" s="1">
+        <v>285.89999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="1">
         <v>237.31</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="1">
         <v>361.38</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="1">
         <v>317.3</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="1">
         <v>325.99</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="1">
         <v>382.6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A9" s="8">
+    <row r="9" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="1">
         <v>229.73</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="1">
         <v>349.88</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="1">
         <v>333.21</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="1">
         <v>435.97</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="1">
         <v>505.78</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="1">
         <v>450.3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A10" s="8">
+    <row r="10" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="1">
         <v>285.3</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="1">
         <v>355.63</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="1">
         <v>193.23</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="1">
         <v>361.57</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="1">
         <v>505.78</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="1">
         <v>336.25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A11" s="8">
+    <row r="11" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="1">
         <v>285.3</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="1">
         <v>361.38</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="1">
         <v>377.75</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="1">
         <v>371.28</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="1">
         <v>388.6</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="1">
         <v>411.62</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A12" s="8">
+    <row r="12" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="9">
-        <v>277.72</v>
-      </c>
-      <c r="C12" s="8">
+      <c r="B12" s="1">
+        <v>277.72000000000003</v>
+      </c>
+      <c r="C12" s="1">
         <v>347</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="1">
         <v>368.21</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="1">
         <v>377.75</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="1">
         <v>463.46</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="1">
         <v>440.63</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A13" s="8">
+    <row r="13" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="1">
         <v>280.25</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="1">
         <v>321.13</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="1">
         <v>272.77</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="1">
         <v>426.26</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="1">
         <v>486.25</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="1">
         <v>189.2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A14" s="8">
+    <row r="14" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="1">
         <v>275.2</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="1">
         <v>341.25</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="1">
         <v>317.3</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="1">
         <v>442.44</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="1">
         <v>489.5</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="1">
         <v>189.2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A15" s="8">
+    <row r="15" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="1">
         <v>280.25</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="1">
         <v>321.13</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="1">
         <v>431.83</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="1">
         <v>468.31</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="1">
         <v>476.48</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="1">
         <v>189.2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A16" s="8">
+    <row r="16" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="1">
         <v>282.77</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="1">
         <v>338.38</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="1">
         <v>441.38</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="1">
         <v>452.14</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="1">
         <v>476.48</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="1">
         <v>405.17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A17" s="8">
+    <row r="17" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="1">
         <v>285.3</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="1">
         <v>349.88</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="1">
         <v>444.56</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="1">
         <v>465.05</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="1">
         <v>382.09</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="1">
         <v>227.88</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A18" s="8">
+    <row r="18" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="1">
         <v>280.25</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="1">
         <v>355.63</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="1">
         <v>428.65</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="1">
         <v>371.28</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="1">
         <v>414.64</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="1">
         <v>421.29</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A19" s="8">
+    <row r="19" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="1">
         <v>287.82</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="1">
         <v>370</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="1">
         <v>387.29</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="1">
         <v>461.85</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="1">
         <v>320.25</v>
       </c>
-      <c r="G19" s="9">
-        <v>314.91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A20" s="8">
+      <c r="G19" s="1">
+        <v>314.91000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="1">
         <v>285.3</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="1">
         <v>341.25</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="1">
         <v>275.95</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="1">
         <v>465.08</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="1">
         <v>408.13</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="1">
         <v>350.37</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A21" s="8">
+    <row r="21" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="1">
         <v>287.82</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="1">
         <v>298.13</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="1">
         <v>419.11</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="1">
         <v>296.88</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="1">
         <v>421.15</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="1">
         <v>224.66</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A22" s="8">
+    <row r="22" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="1">
         <v>282.77</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="1">
         <v>275.13</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="1">
         <v>180.51</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="1">
         <v>371.28</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="1">
         <v>489.5</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="1">
         <v>276.23</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A23" s="8">
+    <row r="23" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="1">
         <v>285.3</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="1">
         <v>352.75</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="1">
         <v>435.01</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="1">
         <v>258.07</v>
       </c>
-      <c r="F23" s="11">
-        <v>46.346</v>
-      </c>
-      <c r="G23" s="9">
+      <c r="F23" s="1">
+        <v>46.345999999999997</v>
+      </c>
+      <c r="G23" s="1">
         <v>218.21</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A24" s="8">
+    <row r="24" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="1">
         <v>280.25</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="1">
         <v>329.75</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="1">
         <v>419.11</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="1">
         <v>190.14</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="1">
         <v>486.25</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="1">
         <v>385.83</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A25" s="8">
+    <row r="25" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="1">
         <v>285.3</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="1">
         <v>289.5</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="1">
         <v>422.29</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="1">
         <v>235.42</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="1">
         <v>460.21</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="1">
         <v>427.73</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A26" s="8">
+    <row r="26" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="1">
         <v>285.3</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="1">
         <v>375.75</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="1">
         <v>396.84</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="1">
         <v>209.55</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="1">
         <v>473.23</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="1">
         <v>392.27</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A27" s="8">
+    <row r="27" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="1">
         <v>287.82</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="1">
         <v>384.38</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="1">
         <v>403.2</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="1">
         <v>448.91</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="1">
         <v>476.48</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="1">
         <v>369.71</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A28" s="8">
+    <row r="28" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="1">
         <v>292.88</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="1">
         <v>387.25</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="1">
         <v>409.56</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="1">
         <v>416.56</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="1">
         <v>463.46</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="1">
         <v>360.04</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A29" s="8">
+    <row r="29" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="1">
         <v>252.46</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="1">
         <v>364.25</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="1">
         <v>400.02</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="1">
         <v>435.97</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="1">
         <v>473.23</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="1">
         <v>385.83</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A30" s="8">
+    <row r="30" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="1">
         <v>275.2</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="1">
         <v>375.75</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="1">
         <v>374.57</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="1">
         <v>426.26</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="1">
         <v>450.44</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="1">
         <v>350.37</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A31" s="8">
+    <row r="31" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="1">
         <v>229.93</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="9">
+      <c r="D31" s="1">
         <v>361.84</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="1">
         <v>478.08</v>
       </c>
-      <c r="F31" s="10">
+      <c r="F31" s="1">
         <v>186.8</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="1">
         <v>392.27</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A32" s="8">
+    <row r="32" spans="1:7" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="1">
         <v>300.45</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="9">
+      <c r="D32" s="1">
         <v>447.74</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="1">
         <v>468.31</v>
       </c>
-      <c r="F32" s="10">
+      <c r="F32" s="1">
         <v>186.8</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="1">
         <v>221.43</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="9.50" customHeight="1">
-      <c r="A33" s="8">
+    <row r="33" spans="1:6" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="1">
         <v>300.45</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="9">
+      <c r="D33" s="1">
         <v>431.83</v>
       </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="9">
+      <c r="F33" s="1">
         <v>336.52</v>
       </c>
-      <c r="G33" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>